<commit_message>
updateSelectInput added for localities reading an excel file
</commit_message>
<xml_diff>
--- a/inst/hidap/sites/Master-list-trial-sites.xlsx
+++ b/inst/hidap/sites/Master-list-trial-sites.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Admin names" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sites!$A$1:$S$113</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sites!$M$1:$M$115</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -246,7 +246,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="955">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2287" uniqueCount="951">
   <si>
     <t>Embargo till</t>
   </si>
@@ -3077,21 +3077,6 @@
     <t>Khokhri</t>
   </si>
   <si>
-    <t>114</t>
-  </si>
-  <si>
-    <t>OPRL</t>
-  </si>
-  <si>
-    <t>operal</t>
-  </si>
-  <si>
-    <t>Andorra</t>
-  </si>
-  <si>
-    <t>opjyyy</t>
-  </si>
-  <si>
     <t>115</t>
   </si>
   <si>
@@ -3111,6 +3096,9 @@
   </si>
   <si>
     <t>2612.0</t>
+  </si>
+  <si>
+    <t>San Ramon-2</t>
   </si>
 </sst>
 </file>
@@ -3629,13 +3617,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S116"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:S115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G100" sqref="G100"/>
+      <selection pane="bottomRight" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3720,7 +3709,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>86</v>
       </c>
@@ -3911,7 +3900,7 @@
         <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>950</v>
       </c>
       <c r="F5" t="s">
         <v>528</v>
@@ -4428,7 +4417,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>837</v>
       </c>
@@ -4487,7 +4476,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>838</v>
       </c>
@@ -4546,7 +4535,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>839</v>
       </c>
@@ -4605,7 +4594,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="17" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>840</v>
       </c>
@@ -4664,7 +4653,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>841</v>
       </c>
@@ -4723,7 +4712,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="19" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>842</v>
       </c>
@@ -4782,7 +4771,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="20" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>843</v>
       </c>
@@ -4841,7 +4830,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="21" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>844</v>
       </c>
@@ -4900,7 +4889,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="22" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>845</v>
       </c>
@@ -4959,7 +4948,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="23" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:19" ht="15.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>846</v>
       </c>
@@ -5018,7 +5007,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="24" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>518</v>
       </c>
@@ -5077,7 +5066,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="25" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>847</v>
       </c>
@@ -5136,7 +5125,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>848</v>
       </c>
@@ -5195,7 +5184,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="27" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>849</v>
       </c>
@@ -5254,7 +5243,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="28" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>850</v>
       </c>
@@ -5313,7 +5302,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="29" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>851</v>
       </c>
@@ -5372,7 +5361,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>852</v>
       </c>
@@ -5431,7 +5420,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>853</v>
       </c>
@@ -5490,7 +5479,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>854</v>
       </c>
@@ -5549,7 +5538,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>855</v>
       </c>
@@ -5608,7 +5597,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>856</v>
       </c>
@@ -5667,7 +5656,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>857</v>
       </c>
@@ -5726,7 +5715,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="36" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>858</v>
       </c>
@@ -5785,7 +5774,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="37" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>859</v>
       </c>
@@ -5844,7 +5833,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="38" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>860</v>
       </c>
@@ -5903,7 +5892,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="39" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>861</v>
       </c>
@@ -5962,7 +5951,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="40" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>862</v>
       </c>
@@ -6021,7 +6010,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="41" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>863</v>
       </c>
@@ -6080,7 +6069,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>864</v>
       </c>
@@ -6139,7 +6128,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="43" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>865</v>
       </c>
@@ -6198,7 +6187,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="44" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>866</v>
       </c>
@@ -6257,7 +6246,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="45" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>867</v>
       </c>
@@ -6316,7 +6305,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="46" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>868</v>
       </c>
@@ -6375,7 +6364,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="47" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>869</v>
       </c>
@@ -6434,7 +6423,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="48" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>870</v>
       </c>
@@ -6493,7 +6482,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="49" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>871</v>
       </c>
@@ -6552,7 +6541,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>872</v>
       </c>
@@ -6611,7 +6600,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="51" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>873</v>
       </c>
@@ -6670,7 +6659,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="52" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>874</v>
       </c>
@@ -6729,7 +6718,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="53" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>875</v>
       </c>
@@ -6788,7 +6777,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="54" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>876</v>
       </c>
@@ -6847,7 +6836,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="55" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>877</v>
       </c>
@@ -6906,7 +6895,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>878</v>
       </c>
@@ -6965,7 +6954,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>879</v>
       </c>
@@ -7024,7 +7013,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="58" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>880</v>
       </c>
@@ -7083,7 +7072,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="59" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>881</v>
       </c>
@@ -7142,7 +7131,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="60" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>519</v>
       </c>
@@ -7201,7 +7190,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="61" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>882</v>
       </c>
@@ -7260,7 +7249,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="62" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>883</v>
       </c>
@@ -7319,7 +7308,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="63" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>884</v>
       </c>
@@ -7378,7 +7367,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="64" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>885</v>
       </c>
@@ -7437,7 +7426,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="65" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>886</v>
       </c>
@@ -7496,7 +7485,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="66" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>520</v>
       </c>
@@ -7555,7 +7544,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="67" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>887</v>
       </c>
@@ -7614,7 +7603,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="68" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>888</v>
       </c>
@@ -7673,7 +7662,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="69" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>889</v>
       </c>
@@ -7732,7 +7721,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="70" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>521</v>
       </c>
@@ -7791,7 +7780,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="71" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>890</v>
       </c>
@@ -7850,7 +7839,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="72" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>891</v>
       </c>
@@ -7909,7 +7898,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="73" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>892</v>
       </c>
@@ -7968,7 +7957,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="74" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>893</v>
       </c>
@@ -8027,7 +8016,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="75" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>894</v>
       </c>
@@ -8086,7 +8075,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="76" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>895</v>
       </c>
@@ -8145,7 +8134,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="77" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>896</v>
       </c>
@@ -8204,7 +8193,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="78" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>897</v>
       </c>
@@ -8794,7 +8783,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="88" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>906</v>
       </c>
@@ -8853,7 +8842,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="89" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>907</v>
       </c>
@@ -8912,7 +8901,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="90" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>908</v>
       </c>
@@ -8971,7 +8960,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="91" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>909</v>
       </c>
@@ -9030,7 +9019,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="92" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>910</v>
       </c>
@@ -9089,7 +9078,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="93" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>911</v>
       </c>
@@ -9148,7 +9137,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="94" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>912</v>
       </c>
@@ -9207,7 +9196,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="95" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>913</v>
       </c>
@@ -9266,7 +9255,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="96" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>914</v>
       </c>
@@ -9325,7 +9314,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="97" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>915</v>
       </c>
@@ -9384,7 +9373,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="98" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>916</v>
       </c>
@@ -9443,7 +9432,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="99" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>917</v>
       </c>
@@ -9502,7 +9491,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="100" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>918</v>
       </c>
@@ -9561,7 +9550,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="101" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>919</v>
       </c>
@@ -9620,7 +9609,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="102" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>920</v>
       </c>
@@ -9679,7 +9668,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="103" spans="1:19" s="8" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:19" s="8" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>921</v>
       </c>
@@ -9738,7 +9727,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="104" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>922</v>
       </c>
@@ -9797,7 +9786,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="105" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>923</v>
       </c>
@@ -9856,7 +9845,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="106" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>924</v>
       </c>
@@ -9915,7 +9904,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="107" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>925</v>
       </c>
@@ -9974,7 +9963,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="108" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>926</v>
       </c>
@@ -10033,7 +10022,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="109" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>927</v>
       </c>
@@ -10092,7 +10081,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="110" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>928</v>
       </c>
@@ -10151,7 +10140,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="111" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>929</v>
       </c>
@@ -10210,7 +10199,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="112" spans="1:19" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:19" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>930</v>
       </c>
@@ -10269,7 +10258,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="113" spans="1:19" s="9" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:19" s="9" customFormat="1" ht="12.75" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>931</v>
       </c>
@@ -10328,7 +10317,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="114" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:19" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>932</v>
       </c>
@@ -10401,16 +10390,16 @@
         <v>945</v>
       </c>
       <c r="E115" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="F115" t="s">
-        <v>840</v>
+        <v>947</v>
       </c>
       <c r="G115" t="s">
-        <v>849</v>
+        <v>948</v>
       </c>
       <c r="H115" t="s">
-        <v>850</v>
+        <v>949</v>
       </c>
       <c r="I115" t="s">
         <v>939</v>
@@ -10419,13 +10408,13 @@
         <v>525</v>
       </c>
       <c r="K115" t="s">
-        <v>264</v>
+        <v>143</v>
       </c>
       <c r="L115" t="s">
-        <v>206</v>
+        <v>141</v>
       </c>
       <c r="M115" t="s">
-        <v>946</v>
+        <v>45</v>
       </c>
       <c r="N115" s="12" t="s">
         <v>525</v>
@@ -10437,7 +10426,7 @@
         <v>525</v>
       </c>
       <c r="Q115" s="12" t="s">
-        <v>947</v>
+        <v>525</v>
       </c>
       <c r="R115" t="s">
         <v>117</v>
@@ -10446,66 +10435,14 @@
         <v>525</v>
       </c>
     </row>
-    <row r="116" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A116" t="s">
-        <v>948</v>
-      </c>
-      <c r="B116" t="s">
-        <v>949</v>
-      </c>
-      <c r="C116" t="s">
-        <v>525</v>
-      </c>
-      <c r="D116" t="s">
-        <v>950</v>
-      </c>
-      <c r="E116" t="s">
-        <v>951</v>
-      </c>
-      <c r="F116" t="s">
-        <v>952</v>
-      </c>
-      <c r="G116" t="s">
-        <v>953</v>
-      </c>
-      <c r="H116" t="s">
-        <v>954</v>
-      </c>
-      <c r="I116" t="s">
-        <v>939</v>
-      </c>
-      <c r="J116" t="s">
-        <v>525</v>
-      </c>
-      <c r="K116" t="s">
-        <v>143</v>
-      </c>
-      <c r="L116" t="s">
-        <v>141</v>
-      </c>
-      <c r="M116" t="s">
-        <v>45</v>
-      </c>
-      <c r="N116" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="O116" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="P116" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="Q116" s="12" t="s">
-        <v>525</v>
-      </c>
-      <c r="R116" t="s">
-        <v>117</v>
-      </c>
-      <c r="S116" t="s">
-        <v>525</v>
-      </c>
-    </row>
   </sheetData>
+  <autoFilter ref="M1:M115">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="Peru"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:S143">
     <sortCondition ref="A2:A143"/>
   </sortState>

</xml_diff>